<commit_message>
Add common skill Hymn of Patience
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20339"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Stuff\Coding\ModdingSlayTheSpire\my_mods\git\StS-DefaultModBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\my_mods\theForsaken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4D4958-2D4A-4279-92AE-904F3C9F1E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="278" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21156" windowHeight="12300" tabRatio="278"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_Hlk529464078" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Common</t>
   </si>
@@ -92,12 +91,15 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>Mine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,7 +213,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,6 +239,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -244,15 +258,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -264,7 +269,10 @@
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -282,9 +290,14 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -310,18 +323,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -338,9 +341,23 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -366,24 +383,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -400,9 +401,14 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -434,7 +440,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -482,9 +487,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gremy Simple Dark" pivot="0" count="2" xr9:uid="{588A353C-8878-412F-8D27-6178F08779F5}">
-      <tableStyleElement type="wholeTable" dxfId="31"/>
-      <tableStyleElement type="headerRow" dxfId="30"/>
+    <tableStyle name="Gremy Simple Dark" pivot="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -507,49 +512,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2121A485-2482-4860-9E30-DE2D287A6F7A}" name="Table2" displayName="Table2" ref="A6:D13" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A6:D12" xr:uid="{D21865EF-8925-4FB2-A04B-9FCEFE947069}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:E13" totalsRowCount="1" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A6:E12">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Cost" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Mine" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(Table2[Mine])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="F6:I10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Cost" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="F6:I10" xr:uid="{CE12703D-A0E8-4EAA-9688-E5928D5B5BFB}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Rarity" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FEC834A-9605-4DAB-8FC8-559DFE95E7CE}" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="F16:I19" xr:uid="{AB9EBA6F-19E5-4878-B4BF-640070BDE1CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="F16:I19"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{10488BD1-9981-44C8-B679-8617EA80CFDF}" name="Type" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2BD6E313-819A-4120-B615-A73747A8BFF9}" name="Silent" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{29092D1A-1D35-4F6E-9938-E644E403DC81}" name="Ironclad" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D8133038-6E03-4174-95AC-6C4D249B7298}" name="Defect" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Type" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,62 +859,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7173905A-9702-4724-9D18-DFCD7AC58563}">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.42578125" style="4"/>
+    <col min="1" max="9" width="12.44140625" style="4"/>
+    <col min="10" max="10" width="12.44140625" style="9"/>
+    <col min="11" max="16384" width="12.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -919,6 +930,9 @@
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E6" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
@@ -931,8 +945,11 @@
       <c r="I6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -945,6 +962,9 @@
       <c r="D7" s="4">
         <v>3</v>
       </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
@@ -957,8 +977,11 @@
       <c r="I7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -971,6 +994,9 @@
       <c r="D8" s="4">
         <v>12</v>
       </c>
+      <c r="E8" s="9">
+        <v>6</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>0</v>
       </c>
@@ -983,8 +1009,11 @@
       <c r="I8" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -997,6 +1026,9 @@
       <c r="D9" s="4">
         <v>43</v>
       </c>
+      <c r="E9" s="9">
+        <v>18</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1009,8 +1041,11 @@
       <c r="I9" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -1023,6 +1058,9 @@
       <c r="D10" s="4">
         <v>11</v>
       </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
       </c>
@@ -1035,8 +1073,11 @@
       <c r="I10" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -1048,6 +1089,9 @@
       </c>
       <c r="D11" s="4">
         <v>4</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>10</v>
@@ -1064,8 +1108,12 @@
         <f>SUBTOTAL(109,Table24[Defect])</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="5">
+        <f>SUM(J7:J10)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1078,8 +1126,11 @@
       <c r="D12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1095,26 +1146,31 @@
         <f>SUBTOTAL(109,Table2[Defect])</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="E13" s="5">
+        <f>SUM(Table2[Mine])</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="9" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
       <c r="F16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1127,13 +1183,16 @@
       <c r="I16" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="F17" s="12" t="s">
+      <c r="J16" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="4">
@@ -1145,11 +1204,14 @@
       <c r="I17" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="4">
@@ -1161,11 +1223,14 @@
       <c r="I18" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="4">
@@ -1177,8 +1242,11 @@
       <c r="I19" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="F20" s="5" t="s">
@@ -1196,23 +1264,27 @@
         <f>SUBTOTAL(109,Table242[Defect])</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="5">
+        <f>SUM(J17:J19)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G30" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix unplayed card variable for compendium.
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Common</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>Mine</t>
+  </si>
+  <si>
+    <t>3 @ -2</t>
+  </si>
+  <si>
+    <t>~10</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>~5</t>
+  </si>
+  <si>
+    <t>~7-8</t>
+  </si>
+  <si>
+    <t>~15</t>
+  </si>
+  <si>
+    <t>~1-3</t>
   </si>
 </sst>
 </file>
@@ -116,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,6 +231,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -213,7 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -258,6 +300,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -307,9 +355,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -403,6 +448,9 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -524,7 +572,7 @@
     <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="3"/>
     <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="2"/>
     <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="Mine" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="0">
+    <tableColumn id="5" name="Mine" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="0">
       <totalsRowFormula>SUM(Table2[Mine])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -533,7 +581,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="F6:I10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -541,23 +589,23 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="F16:I19"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Type" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="1" name="Type" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Silent" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Ironclad" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Defect" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -860,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +921,7 @@
     <col min="11" max="16384" width="12.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
@@ -884,7 +932,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -893,7 +941,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -902,7 +950,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -917,7 +965,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -945,11 +993,11 @@
       <c r="I6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -963,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
@@ -977,11 +1025,14 @@
       <c r="I7" s="4">
         <v>4</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="17">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -1009,11 +1060,14 @@
       <c r="I8" s="4">
         <v>18</v>
       </c>
-      <c r="J8" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="17">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1027,7 +1081,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="9">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>1</v>
@@ -1041,11 +1095,14 @@
       <c r="I9" s="4">
         <v>36</v>
       </c>
-      <c r="J9" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="17">
+        <v>23</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -1059,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="9">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
@@ -1073,11 +1130,14 @@
       <c r="I10" s="4">
         <v>17</v>
       </c>
-      <c r="J10" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="17">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -1091,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>10</v>
@@ -1108,12 +1168,15 @@
         <f>SUBTOTAL(109,Table24[Defect])</f>
         <v>75</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="17">
         <f>SUM(J7:J10)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="K11" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1148,16 +1211,19 @@
       </c>
       <c r="E13" s="5">
         <f>SUM(Table2[Mine])</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
+      <c r="E15" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
@@ -1166,7 +1232,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1183,11 +1249,11 @@
       <c r="I16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1204,11 +1270,14 @@
       <c r="I17" s="4">
         <v>24</v>
       </c>
-      <c r="J17" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="17">
+        <v>18</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="F18" s="11" t="s">
@@ -1223,11 +1292,14 @@
       <c r="I18" s="4">
         <v>37</v>
       </c>
-      <c r="J18" s="9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="17">
+        <v>21</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="F19" s="12" t="s">
@@ -1242,11 +1314,14 @@
       <c r="I19" s="4">
         <v>14</v>
       </c>
-      <c r="J19" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J19" s="17">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="F20" s="5" t="s">
@@ -1264,27 +1339,27 @@
         <f>SUBTOTAL(109,Table242[Defect])</f>
         <v>75</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="17">
         <f>SUM(J17:J19)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G30" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add uncommon skill Bottled Plague
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Common</t>
   </si>
@@ -99,22 +99,13 @@
     <t>3 @ -2</t>
   </si>
   <si>
-    <t>~10</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>~5</t>
-  </si>
-  <si>
     <t>~7-8</t>
   </si>
   <si>
     <t>~15</t>
-  </si>
-  <si>
-    <t>~1-3</t>
   </si>
 </sst>
 </file>
@@ -293,6 +284,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -300,12 +297,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -910,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,47 +913,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -993,7 +984,7 @@
       <c r="I6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1025,11 +1016,11 @@
       <c r="I7" s="4">
         <v>4</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="14">
         <v>4</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1046,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>0</v>
@@ -1060,8 +1051,8 @@
       <c r="I8" s="4">
         <v>18</v>
       </c>
-      <c r="J8" s="17">
-        <v>9</v>
+      <c r="J8" s="14">
+        <v>20</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>23</v>
@@ -1081,7 +1072,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="9">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>1</v>
@@ -1095,11 +1086,11 @@
       <c r="I9" s="4">
         <v>36</v>
       </c>
-      <c r="J9" s="17">
-        <v>23</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>23</v>
+      <c r="J9" s="14">
+        <v>25</v>
+      </c>
+      <c r="K9" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1116,7 +1107,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
@@ -1130,11 +1121,11 @@
       <c r="I10" s="4">
         <v>17</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>14</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>25</v>
+      <c r="K10" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1168,12 +1159,12 @@
         <f>SUBTOTAL(109,Table24[Defect])</f>
         <v>75</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="14">
         <f>SUM(J7:J10)</f>
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K11" s="4">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1211,32 +1202,32 @@
       </c>
       <c r="E13" s="5">
         <f>SUM(Table2[Mine])</f>
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="F16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1249,15 +1240,15 @@
       <c r="I16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
       <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
@@ -1270,11 +1261,11 @@
       <c r="I17" s="4">
         <v>24</v>
       </c>
-      <c r="J17" s="17">
-        <v>18</v>
+      <c r="J17" s="14">
+        <v>22</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1292,11 +1283,11 @@
       <c r="I18" s="4">
         <v>37</v>
       </c>
-      <c r="J18" s="17">
-        <v>21</v>
+      <c r="J18" s="14">
+        <v>28</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1314,11 +1305,11 @@
       <c r="I19" s="4">
         <v>14</v>
       </c>
-      <c r="J19" s="17">
-        <v>11</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>28</v>
+      <c r="J19" s="14">
+        <v>13</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1339,9 +1330,9 @@
         <f>SUBTOTAL(109,Table242[Defect])</f>
         <v>75</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="14">
         <f>SUM(J17:J19)</f>
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add rare attack Confusion
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -902,7 +902,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1087,7 @@
         <v>36</v>
       </c>
       <c r="J9" s="14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K9" s="4">
         <v>9</v>
@@ -1107,7 +1107,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="J11" s="14">
         <f>SUM(J7:J10)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K11" s="4">
         <v>13</v>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="E13" s="5">
         <f>SUM(Table2[Mine])</f>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1284,7 +1284,7 @@
         <v>37</v>
       </c>
       <c r="J18" s="14">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>25</v>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="J20" s="14">
         <f>SUM(J17:J19)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>